<commit_message>
[multiple changes for production]: production ready code
</commit_message>
<xml_diff>
--- a/server/excel/entries.xlsx
+++ b/server/excel/entries.xlsx
@@ -28,16 +28,16 @@
     <t>Hobbies</t>
   </si>
   <si>
-    <t>angkush-2</t>
+    <t>another one</t>
   </si>
   <si>
     <t>angkush@gmail.com</t>
   </si>
   <si>
-    <t>8876690053</t>
-  </si>
-  <si>
-    <t>hobby-2</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>something</t>
   </si>
 </sst>
 </file>

</xml_diff>